<commit_message>
Update Keras Hyperband Optimizer
</commit_message>
<xml_diff>
--- a/datasets/DOE_Full_Factorial.xlsx
+++ b/datasets/DOE_Full_Factorial.xlsx
@@ -408,13 +408,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>80.40036015459947</v>
       </c>
       <c r="C2">
-        <v>0.0009999999999999454</v>
+        <v>0.08040036015459946</v>
       </c>
       <c r="D2">
-        <v>0.00083</v>
+        <v>0.0008040036015459946</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -422,13 +422,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>1000</v>
+        <v>119.5996398454005</v>
       </c>
       <c r="C3">
-        <v>0.0009999999999999454</v>
+        <v>0.08040036015459946</v>
       </c>
       <c r="D3">
-        <v>0.00083</v>
+        <v>0.0008040036015459946</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -436,13 +436,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>10</v>
+        <v>80.40036015459947</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0.1195996398454005</v>
       </c>
       <c r="D4">
-        <v>0.00083</v>
+        <v>0.0008040036015459946</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>1000</v>
+        <v>119.5996398454005</v>
       </c>
       <c r="C5">
-        <v>1</v>
+        <v>0.1195996398454005</v>
       </c>
       <c r="D5">
-        <v>0.00083</v>
+        <v>0.0008040036015459946</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>10</v>
+        <v>80.40036015459947</v>
       </c>
       <c r="C6">
-        <v>0.0009999999999999454</v>
+        <v>0.08040036015459946</v>
       </c>
       <c r="D6">
-        <v>0.002</v>
+        <v>0.001195996398454005</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>1000</v>
+        <v>119.5996398454005</v>
       </c>
       <c r="C7">
-        <v>0.0009999999999999454</v>
+        <v>0.08040036015459946</v>
       </c>
       <c r="D7">
-        <v>0.002</v>
+        <v>0.001195996398454005</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>10</v>
+        <v>80.40036015459947</v>
       </c>
       <c r="C8">
-        <v>1</v>
+        <v>0.1195996398454005</v>
       </c>
       <c r="D8">
-        <v>0.002</v>
+        <v>0.001195996398454005</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>1000</v>
+        <v>119.5996398454005</v>
       </c>
       <c r="C9">
-        <v>1</v>
+        <v>0.1195996398454005</v>
       </c>
       <c r="D9">
-        <v>0.002</v>
+        <v>0.001195996398454005</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update DOE - Add Read Files and Add Lines
</commit_message>
<xml_diff>
--- a/datasets/DOE_Full_Factorial.xlsx
+++ b/datasets/DOE_Full_Factorial.xlsx
@@ -408,7 +408,7 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>80.40036015459947</v>
+        <v>98.04003601545995</v>
       </c>
       <c r="C2">
         <v>0.08040036015459946</v>
@@ -422,7 +422,7 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>119.5996398454005</v>
+        <v>101.9599639845401</v>
       </c>
       <c r="C3">
         <v>0.08040036015459946</v>
@@ -436,7 +436,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>80.40036015459947</v>
+        <v>98.04003601545995</v>
       </c>
       <c r="C4">
         <v>0.1195996398454005</v>
@@ -450,7 +450,7 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>119.5996398454005</v>
+        <v>101.9599639845401</v>
       </c>
       <c r="C5">
         <v>0.1195996398454005</v>
@@ -464,7 +464,7 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>80.40036015459947</v>
+        <v>98.04003601545995</v>
       </c>
       <c r="C6">
         <v>0.08040036015459946</v>
@@ -478,7 +478,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>119.5996398454005</v>
+        <v>101.9599639845401</v>
       </c>
       <c r="C7">
         <v>0.08040036015459946</v>
@@ -492,7 +492,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>80.40036015459947</v>
+        <v>98.04003601545995</v>
       </c>
       <c r="C8">
         <v>0.1195996398454005</v>
@@ -506,7 +506,7 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>119.5996398454005</v>
+        <v>101.9599639845401</v>
       </c>
       <c r="C9">
         <v>0.1195996398454005</v>

</xml_diff>

<commit_message>
Add Setups and Results
</commit_message>
<xml_diff>
--- a/datasets/DOE_Full_Factorial.xlsx
+++ b/datasets/DOE_Full_Factorial.xlsx
@@ -408,13 +408,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>98.04003601545995</v>
+        <v>10</v>
       </c>
       <c r="C2">
-        <v>0.08040036015459946</v>
+        <v>0.0009999999999999454</v>
       </c>
       <c r="D2">
-        <v>0.0008040036015459946</v>
+        <v>0.00083</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -422,13 +422,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>101.9599639845401</v>
+        <v>1000</v>
       </c>
       <c r="C3">
-        <v>0.08040036015459946</v>
+        <v>0.0009999999999999454</v>
       </c>
       <c r="D3">
-        <v>0.0008040036015459946</v>
+        <v>0.00083</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -436,13 +436,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>98.04003601545995</v>
+        <v>10</v>
       </c>
       <c r="C4">
-        <v>0.1195996398454005</v>
+        <v>1</v>
       </c>
       <c r="D4">
-        <v>0.0008040036015459946</v>
+        <v>0.00083</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>101.9599639845401</v>
+        <v>1000</v>
       </c>
       <c r="C5">
-        <v>0.1195996398454005</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.0008040036015459946</v>
+        <v>0.00083</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>98.04003601545995</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>0.08040036015459946</v>
+        <v>0.0009999999999999454</v>
       </c>
       <c r="D6">
-        <v>0.001195996398454005</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>101.9599639845401</v>
+        <v>1000</v>
       </c>
       <c r="C7">
-        <v>0.08040036015459946</v>
+        <v>0.0009999999999999454</v>
       </c>
       <c r="D7">
-        <v>0.001195996398454005</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>98.04003601545995</v>
+        <v>10</v>
       </c>
       <c r="C8">
-        <v>0.1195996398454005</v>
+        <v>1</v>
       </c>
       <c r="D8">
-        <v>0.001195996398454005</v>
+        <v>0.002</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>101.9599639845401</v>
+        <v>1000</v>
       </c>
       <c r="C9">
-        <v>0.1195996398454005</v>
+        <v>1</v>
       </c>
       <c r="D9">
-        <v>0.001195996398454005</v>
+        <v>0.002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Test with Discrete DOE
</commit_message>
<xml_diff>
--- a/datasets/DOE_Full_Factorial.xlsx
+++ b/datasets/DOE_Full_Factorial.xlsx
@@ -408,13 +408,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>80.40036015459947</v>
+        <v>70</v>
       </c>
       <c r="C2">
-        <v>0.08040036015459946</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D2">
-        <v>0.0008040036015459946</v>
+        <v>0.0007000000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -422,13 +422,13 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>119.5996398454005</v>
+        <v>130</v>
       </c>
       <c r="C3">
-        <v>0.08040036015459946</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D3">
-        <v>0.0008040036015459946</v>
+        <v>0.0007000000000000001</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -436,13 +436,13 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>80.40036015459947</v>
+        <v>70</v>
       </c>
       <c r="C4">
-        <v>0.1195996398454005</v>
+        <v>0.13</v>
       </c>
       <c r="D4">
-        <v>0.0008040036015459946</v>
+        <v>0.0007000000000000001</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -450,13 +450,13 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>119.5996398454005</v>
+        <v>130</v>
       </c>
       <c r="C5">
-        <v>0.1195996398454005</v>
+        <v>0.13</v>
       </c>
       <c r="D5">
-        <v>0.0008040036015459946</v>
+        <v>0.0007000000000000001</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -464,13 +464,13 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>80.40036015459947</v>
+        <v>70</v>
       </c>
       <c r="C6">
-        <v>0.08040036015459946</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D6">
-        <v>0.001195996398454005</v>
+        <v>0.0013</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -478,13 +478,13 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>119.5996398454005</v>
+        <v>130</v>
       </c>
       <c r="C7">
-        <v>0.08040036015459946</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="D7">
-        <v>0.001195996398454005</v>
+        <v>0.0013</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -492,13 +492,13 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>80.40036015459947</v>
+        <v>70</v>
       </c>
       <c r="C8">
-        <v>0.1195996398454005</v>
+        <v>0.13</v>
       </c>
       <c r="D8">
-        <v>0.001195996398454005</v>
+        <v>0.0013</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -506,13 +506,13 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>119.5996398454005</v>
+        <v>130</v>
       </c>
       <c r="C9">
-        <v>0.1195996398454005</v>
+        <v>0.13</v>
       </c>
       <c r="D9">
-        <v>0.001195996398454005</v>
+        <v>0.0013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>